<commit_message>
first version of the model
</commit_message>
<xml_diff>
--- a/BDD.xlsx
+++ b/BDD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charl\solar-data-china\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2D5593-3DA7-49A7-A8DE-DACC964640BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E767DF-1232-4D74-A522-C4C179B0A226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="9960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset" sheetId="1" r:id="rId1"/>
@@ -2376,7 +2376,7 @@
       </c>
       <c r="O5" s="18"/>
     </row>
-    <row r="6" spans="1:15" ht="184.8">
+    <row r="6" spans="1:15" ht="198">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
@@ -3049,9 +3049,9 @@
   </sheetPr>
   <dimension ref="A1:L1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="96" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E3" sqref="E3"/>
+      <selection pane="topRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>